<commit_message>
put opening hours after midnight to the following day
</commit_message>
<xml_diff>
--- a/Utown Outlets Opening Hours.xlsx
+++ b/Utown Outlets Opening Hours.xlsx
@@ -1,33 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bigch\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86677F42-00F7-4228-99F1-81BB46A0581D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$U$26</definedName>
-    <definedName name="Z_2E0E2A39_D75C_4A93_8B9A_DB188D9774FE_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$A$1:$F$26</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$U$26</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_DF95D861_E732_478A_9AD9_C6A3452F328A_.wvu.FilterData">Sheet1!$A$1:$F$26</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView name="Filter 1" guid="{2E0E2A39-D75C-4A93-8B9A-DB188D9774FE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{DF95D861-E732-478A-9AD9-C6A3452F328A}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="107">
   <si>
     <t>Store</t>
   </si>
@@ -107,7 +97,13 @@
     <t>Stephen Riady Centre</t>
   </si>
   <si>
-    <t>1100-0100</t>
+    <t>1100-2359</t>
+  </si>
+  <si>
+    <t>0000-0100, 1100-2359</t>
+  </si>
+  <si>
+    <t>0000-0100, 1100-2200</t>
   </si>
   <si>
     <t>1100-2200</t>
@@ -293,7 +289,16 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>0800-1000</t>
+    <t>0800-2201</t>
+  </si>
+  <si>
+    <t>0800-2202</t>
+  </si>
+  <si>
+    <t>0800-2203</t>
+  </si>
+  <si>
+    <t>0800-2204</t>
   </si>
   <si>
     <t>1100-2000</t>
@@ -302,7 +307,7 @@
     <t>Supersnacks</t>
   </si>
   <si>
-    <t>1200-0200</t>
+    <t>0000-0200, 1200-2359</t>
   </si>
   <si>
     <t>1200-0000</t>
@@ -338,38 +343,27 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <fonts count="6">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+    </font>
+    <font/>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
@@ -379,7 +373,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -389,43 +383,44 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -615,51 +610,48 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="1.0" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B1" sqref="B1" pane="topRight"/>
+      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
+      <selection activeCell="B2" sqref="B2" pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="27.88671875" customWidth="1"/>
-    <col min="7" max="7" width="27.33203125" customWidth="1"/>
-    <col min="8" max="8" width="28" customWidth="1"/>
-    <col min="9" max="9" width="27.44140625" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" customWidth="1"/>
-    <col min="11" max="11" width="27" customWidth="1"/>
-    <col min="12" max="12" width="27.5546875" customWidth="1"/>
-    <col min="13" max="13" width="26.6640625" customWidth="1"/>
-    <col min="14" max="14" width="31.109375" customWidth="1"/>
-    <col min="15" max="15" width="30.44140625" customWidth="1"/>
-    <col min="16" max="16" width="31.109375" customWidth="1"/>
-    <col min="17" max="17" width="30.6640625" customWidth="1"/>
-    <col min="18" max="18" width="29.6640625" customWidth="1"/>
-    <col min="19" max="19" width="30.109375" customWidth="1"/>
-    <col min="20" max="20" width="30.88671875" customWidth="1"/>
-    <col min="21" max="21" width="29.88671875" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="33.43"/>
+    <col customWidth="1" min="2" max="2" width="16.57"/>
+    <col customWidth="1" min="3" max="3" width="17.0"/>
+    <col customWidth="1" min="4" max="4" width="16.43"/>
+    <col customWidth="1" min="5" max="5" width="24.0"/>
+    <col customWidth="1" min="6" max="6" width="27.86"/>
+    <col customWidth="1" min="7" max="7" width="27.29"/>
+    <col customWidth="1" min="8" max="8" width="28.0"/>
+    <col customWidth="1" min="9" max="9" width="27.43"/>
+    <col customWidth="1" min="10" max="10" width="26.43"/>
+    <col customWidth="1" min="11" max="11" width="27.0"/>
+    <col customWidth="1" min="12" max="12" width="27.57"/>
+    <col customWidth="1" min="13" max="13" width="26.71"/>
+    <col customWidth="1" min="14" max="14" width="31.14"/>
+    <col customWidth="1" min="15" max="15" width="30.43"/>
+    <col customWidth="1" min="16" max="16" width="31.14"/>
+    <col customWidth="1" min="17" max="17" width="30.71"/>
+    <col customWidth="1" min="18" max="18" width="29.71"/>
+    <col customWidth="1" min="19" max="19" width="30.14"/>
+    <col customWidth="1" min="20" max="20" width="30.86"/>
+    <col customWidth="1" min="21" max="21" width="29.86"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -724,7 +716,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -740,519 +732,519 @@
       <c r="E2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="H2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="L2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
-      <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="A6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
-      <c r="A7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>52</v>
+      <c r="C8" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="A9" s="3" t="s">
-        <v>54</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>38</v>
+        <v>57</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>52</v>
+      <c r="C10" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>24</v>
@@ -1261,908 +1253,908 @@
         <v>25</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>58</v>
+        <v>38</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
-      <c r="A12" s="3" t="s">
-        <v>60</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
-      <c r="A13" s="3" t="s">
-        <v>63</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="U14" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21">
-      <c r="A15" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>38</v>
+        <v>71</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21">
-      <c r="A18" s="3" t="s">
-        <v>73</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N19" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="O19" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
-      <c r="A21" s="3" t="s">
-        <v>80</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>31</v>
+      <c r="C22" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>88</v>
+      <c r="G23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21">
-      <c r="A24" s="3" t="s">
-        <v>90</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>24</v>
@@ -2170,129 +2162,129 @@
       <c r="E24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>91</v>
+      <c r="F24" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25">
       <c r="A25" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>94</v>
+      <c r="C25" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26">
       <c r="A26" s="2" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>97</v>
+      <c r="C26" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>24</v>
@@ -2301,65 +2293,69 @@
         <v>25</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29">
       <c r="A29" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U26" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="$A$1:$U$26">
+    <sortState ref="A1:U26">
+      <sortCondition ref="A1:A26"/>
+      <sortCondition ref="D1:D26"/>
+    </sortState>
+  </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{2E0E2A39-D75C-4A93-8B9A-DB188D9774FE}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:F26" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
+    <customSheetView guid="{DF95D861-E732-478A-9AD9-C6A3452F328A}" filter="1" showAutoFilter="1">
+      <autoFilter ref="$A$1:$F$26"/>
     </customSheetView>
   </customSheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Edited to focus term opening hours
-Relabelled all opening day headers to just "ddd" (Mon, Tue, etc)
-Edited testbot.py accordingly
</commit_message>
<xml_diff>
--- a/Utown Outlets Opening Hours.xlsx
+++ b/Utown Outlets Opening Hours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Documents\GitHub\NUSUTownTeleBot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bigch\Desktop\GitHub\NUSUTownTeleBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F3CA59-0999-450A-A956-9A4C131FEC44}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A94A26D-E22B-46A7-8ACF-FB048053CA65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,30 +44,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Term Opening Hours (Mon)</t>
-  </si>
-  <si>
-    <t>Term Opening Hours (Tue)</t>
-  </si>
-  <si>
-    <t>Term Opening Hours (Wed)</t>
-  </si>
-  <si>
-    <t>Term Opening Hours (Thu)</t>
-  </si>
-  <si>
-    <t>Term Opening Hours (Fri)</t>
-  </si>
-  <si>
-    <t>Term Opening Hours (Sat)</t>
-  </si>
-  <si>
-    <t>Term Opening Hours (Sun)</t>
-  </si>
-  <si>
-    <t>Term Opening Hours (PH)</t>
-  </si>
-  <si>
     <t>2359 Li Ji Coffeehouse</t>
   </si>
   <si>
@@ -303,13 +279,37 @@
   </si>
   <si>
     <t>Open</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Tue</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>Thu</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>Sat</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>PH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -602,35 +602,35 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="33.46484375" customWidth="1"/>
-    <col min="2" max="2" width="16.53125" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="16.46484375" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="27.86328125" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" customWidth="1"/>
     <col min="7" max="7" width="27.33203125" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
-    <col min="9" max="9" width="27.46484375" customWidth="1"/>
-    <col min="10" max="10" width="26.46484375" customWidth="1"/>
+    <col min="9" max="9" width="27.44140625" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" customWidth="1"/>
     <col min="11" max="11" width="27" customWidth="1"/>
-    <col min="12" max="12" width="27.53125" customWidth="1"/>
+    <col min="12" max="12" width="27.5546875" customWidth="1"/>
     <col min="13" max="13" width="26.6640625" customWidth="1"/>
-    <col min="14" max="14" width="31.1328125" customWidth="1"/>
-    <col min="15" max="15" width="30.46484375" customWidth="1"/>
-    <col min="16" max="16" width="31.1328125" customWidth="1"/>
+    <col min="14" max="14" width="31.109375" customWidth="1"/>
+    <col min="15" max="15" width="30.44140625" customWidth="1"/>
+    <col min="16" max="16" width="31.109375" customWidth="1"/>
     <col min="17" max="17" width="30.6640625" customWidth="1"/>
     <col min="18" max="18" width="29.6640625" customWidth="1"/>
-    <col min="19" max="19" width="30.1328125" customWidth="1"/>
-    <col min="20" max="20" width="30.86328125" customWidth="1"/>
-    <col min="21" max="21" width="29.86328125" customWidth="1"/>
+    <col min="19" max="19" width="30.109375" customWidth="1"/>
+    <col min="20" max="20" width="30.88671875" customWidth="1"/>
+    <col min="21" max="21" width="29.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="13.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,28 +647,28 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>87</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -679,45 +679,45 @@
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="13.2">
       <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="M2" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -728,45 +728,45 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="13.2">
       <c r="A3" s="4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -777,45 +777,45 @@
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" ht="13.2">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -826,45 +826,45 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" ht="13.2">
       <c r="A5" s="4" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -875,45 +875,45 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="13.2">
       <c r="A6" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -924,45 +924,45 @@
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="13.2">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -973,45 +973,45 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="13.2">
       <c r="A8" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -1022,45 +1022,45 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" ht="13.2">
       <c r="A9" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -1071,45 +1071,45 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="13.2">
       <c r="A10" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -1120,45 +1120,45 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" ht="13.2">
       <c r="A11" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1169,45 +1169,45 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" ht="13.2">
       <c r="A12" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1218,45 +1218,45 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" ht="13.2">
       <c r="A13" s="4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1267,45 +1267,45 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" ht="13.2">
       <c r="A14" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -1316,45 +1316,45 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="13.2">
       <c r="A15" s="4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1365,45 +1365,45 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" ht="13.2">
       <c r="A16" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1414,45 +1414,45 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" ht="13.2">
       <c r="A17" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -1463,45 +1463,45 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" ht="13.2">
       <c r="A18" s="4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -1512,45 +1512,45 @@
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" ht="13.2">
       <c r="A19" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -1561,45 +1561,45 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" ht="13.2">
       <c r="A20" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -1610,45 +1610,45 @@
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" ht="13.2">
       <c r="A21" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -1659,45 +1659,45 @@
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="13.2">
       <c r="A22" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -1708,45 +1708,45 @@
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="13.2">
       <c r="A23" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="L23" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -1757,45 +1757,45 @@
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" ht="13.2">
       <c r="A24" s="4" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -1806,45 +1806,45 @@
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" ht="13.2">
       <c r="A25" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -1855,45 +1855,45 @@
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" ht="13.2">
       <c r="A26" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -1904,7 +1904,7 @@
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:21" ht="15.75" customHeight="1">
       <c r="A29" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated timings of all 24/7 stores
-Changed a few leftover ones to 'Open'
</commit_message>
<xml_diff>
--- a/Utown Outlets Opening Hours.xlsx
+++ b/Utown Outlets Opening Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bigch\Desktop\GitHub\NUSUTownTeleBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A94A26D-E22B-46A7-8ACF-FB048053CA65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2ACC835-518B-4B72-AE85-BCED5DC3EE23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="91">
   <si>
     <t>Store</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>Town Plaza</t>
-  </si>
-  <si>
-    <t>0000-2359</t>
   </si>
   <si>
     <t>Collaborative Commons</t>
@@ -599,10 +596,10 @@
   <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -647,28 +644,28 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -843,25 +840,25 @@
         <v>29</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>15</v>
@@ -877,10 +874,10 @@
     </row>
     <row r="6" spans="1:21" ht="13.2">
       <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>24</v>
@@ -889,28 +886,28 @@
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>15</v>
@@ -926,13 +923,13 @@
     </row>
     <row r="7" spans="1:21" ht="13.2">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>24</v>
@@ -941,25 +938,25 @@
         <v>9</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>15</v>
@@ -975,13 +972,13 @@
     </row>
     <row r="8" spans="1:21" ht="13.2">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>8</v>
@@ -990,25 +987,25 @@
         <v>29</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>15</v>
@@ -1024,10 +1021,10 @@
     </row>
     <row r="9" spans="1:21" ht="13.2">
       <c r="A9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>24</v>
@@ -1039,25 +1036,25 @@
         <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>15</v>
@@ -1073,13 +1070,13 @@
     </row>
     <row r="10" spans="1:21" ht="13.2">
       <c r="A10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
@@ -1088,25 +1085,25 @@
         <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>15</v>
@@ -1122,13 +1119,13 @@
     </row>
     <row r="11" spans="1:21" ht="13.2">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>24</v>
@@ -1137,19 +1134,19 @@
         <v>9</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>20</v>
@@ -1171,13 +1168,13 @@
     </row>
     <row r="12" spans="1:21" ht="13.2">
       <c r="A12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>24</v>
@@ -1186,19 +1183,19 @@
         <v>9</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>25</v>
@@ -1220,13 +1217,13 @@
     </row>
     <row r="13" spans="1:21" ht="13.2">
       <c r="A13" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
@@ -1235,22 +1232,22 @@
         <v>29</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>20</v>
@@ -1269,10 +1266,10 @@
     </row>
     <row r="14" spans="1:21" ht="13.2">
       <c r="A14" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>24</v>
@@ -1281,28 +1278,28 @@
         <v>24</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>15</v>
@@ -1318,7 +1315,7 @@
     </row>
     <row r="15" spans="1:21" ht="13.2">
       <c r="A15" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>22</v>
@@ -1333,25 +1330,25 @@
         <v>9</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>15</v>
@@ -1367,10 +1364,10 @@
     </row>
     <row r="16" spans="1:21" ht="13.2">
       <c r="A16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>24</v>
@@ -1382,19 +1379,19 @@
         <v>9</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>20</v>
@@ -1416,10 +1413,10 @@
     </row>
     <row r="17" spans="1:21" ht="13.2">
       <c r="A17" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>24</v>
@@ -1428,28 +1425,28 @@
         <v>24</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>15</v>
@@ -1465,10 +1462,10 @@
     </row>
     <row r="18" spans="1:21" ht="13.2">
       <c r="A18" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>24</v>
@@ -1480,28 +1477,28 @@
         <v>9</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -1514,13 +1511,13 @@
     </row>
     <row r="19" spans="1:21" ht="13.2">
       <c r="A19" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>8</v>
@@ -1563,13 +1560,13 @@
     </row>
     <row r="20" spans="1:21" ht="13.2">
       <c r="A20" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>24</v>
@@ -1578,22 +1575,22 @@
         <v>9</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>20</v>
@@ -1612,13 +1609,13 @@
     </row>
     <row r="21" spans="1:21" ht="13.2">
       <c r="A21" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>24</v>
@@ -1627,19 +1624,19 @@
         <v>9</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>20</v>
@@ -1661,7 +1658,7 @@
     </row>
     <row r="22" spans="1:21" ht="13.2">
       <c r="A22" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -1673,28 +1670,28 @@
         <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>15</v>
@@ -1710,34 +1707,34 @@
     </row>
     <row r="23" spans="1:21" ht="13.2">
       <c r="A23" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>14</v>
@@ -1759,13 +1756,13 @@
     </row>
     <row r="24" spans="1:21" ht="13.2">
       <c r="A24" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>8</v>
@@ -1774,25 +1771,25 @@
         <v>9</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>15</v>
@@ -1808,37 +1805,37 @@
     </row>
     <row r="25" spans="1:21" ht="13.2">
       <c r="A25" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>20</v>
@@ -1857,13 +1854,13 @@
     </row>
     <row r="26" spans="1:21" ht="13.2">
       <c r="A26" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>8</v>
@@ -1872,22 +1869,22 @@
         <v>9</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
return NA if None for API data
</commit_message>
<xml_diff>
--- a/Utown Outlets Opening Hours.xlsx
+++ b/Utown Outlets Opening Hours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bigch\Desktop\GitHub\NUSUTownTeleBot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Documents\GitHub\NUSUTownTeleBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2ACC835-518B-4B72-AE85-BCED5DC3EE23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93F5378-9327-4480-B682-079F117A676B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="4065" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -306,7 +306,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -596,38 +596,38 @@
   <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="33.46484375" customWidth="1"/>
+    <col min="2" max="2" width="16.53125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.46484375" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="27.88671875" customWidth="1"/>
+    <col min="6" max="6" width="27.86328125" customWidth="1"/>
     <col min="7" max="7" width="27.33203125" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
-    <col min="9" max="9" width="27.44140625" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" customWidth="1"/>
+    <col min="9" max="9" width="27.46484375" customWidth="1"/>
+    <col min="10" max="10" width="26.46484375" customWidth="1"/>
     <col min="11" max="11" width="27" customWidth="1"/>
-    <col min="12" max="12" width="27.5546875" customWidth="1"/>
+    <col min="12" max="12" width="27.53125" customWidth="1"/>
     <col min="13" max="13" width="26.6640625" customWidth="1"/>
-    <col min="14" max="14" width="31.109375" customWidth="1"/>
-    <col min="15" max="15" width="30.44140625" customWidth="1"/>
-    <col min="16" max="16" width="31.109375" customWidth="1"/>
+    <col min="14" max="14" width="31.1328125" customWidth="1"/>
+    <col min="15" max="15" width="30.46484375" customWidth="1"/>
+    <col min="16" max="16" width="31.1328125" customWidth="1"/>
     <col min="17" max="17" width="30.6640625" customWidth="1"/>
     <col min="18" max="18" width="29.6640625" customWidth="1"/>
-    <col min="19" max="19" width="30.109375" customWidth="1"/>
-    <col min="20" max="20" width="30.88671875" customWidth="1"/>
-    <col min="21" max="21" width="29.88671875" customWidth="1"/>
+    <col min="19" max="19" width="30.1328125" customWidth="1"/>
+    <col min="20" max="20" width="30.86328125" customWidth="1"/>
+    <col min="21" max="21" width="29.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="13.2">
+    <row r="1" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -676,7 +676,7 @@
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
     </row>
-    <row r="2" spans="1:21" ht="13.2">
+    <row r="2" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -725,7 +725,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:21" ht="13.2">
+    <row r="3" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -774,7 +774,7 @@
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
     </row>
-    <row r="4" spans="1:21" ht="13.2">
+    <row r="4" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -823,7 +823,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
     </row>
-    <row r="5" spans="1:21" ht="13.2">
+    <row r="5" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -872,7 +872,7 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
     </row>
-    <row r="6" spans="1:21" ht="13.2">
+    <row r="6" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -921,7 +921,7 @@
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
     </row>
-    <row r="7" spans="1:21" ht="13.2">
+    <row r="7" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -970,7 +970,7 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
     </row>
-    <row r="8" spans="1:21" ht="13.2">
+    <row r="8" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
@@ -1019,7 +1019,7 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
     </row>
-    <row r="9" spans="1:21" ht="13.2">
+    <row r="9" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>38</v>
       </c>
@@ -1068,7 +1068,7 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="1:21" ht="13.2">
+    <row r="10" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>40</v>
       </c>
@@ -1117,7 +1117,7 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="1:21" ht="13.2">
+    <row r="11" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
@@ -1166,7 +1166,7 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
     </row>
-    <row r="12" spans="1:21" ht="13.2">
+    <row r="12" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>44</v>
       </c>
@@ -1215,7 +1215,7 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="1:21" ht="13.2">
+    <row r="13" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>47</v>
       </c>
@@ -1264,7 +1264,7 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
     </row>
-    <row r="14" spans="1:21" ht="13.2">
+    <row r="14" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
@@ -1313,7 +1313,7 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="1:21" ht="13.2">
+    <row r="15" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>51</v>
       </c>
@@ -1362,7 +1362,7 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="1:21" ht="13.2">
+    <row r="16" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>52</v>
       </c>
@@ -1411,7 +1411,7 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
     </row>
-    <row r="17" spans="1:21" ht="13.2">
+    <row r="17" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>56</v>
       </c>
@@ -1460,7 +1460,7 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
     </row>
-    <row r="18" spans="1:21" ht="13.2">
+    <row r="18" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>57</v>
       </c>
@@ -1509,7 +1509,7 @@
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
     </row>
-    <row r="19" spans="1:21" ht="13.2">
+    <row r="19" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>60</v>
       </c>
@@ -1558,7 +1558,7 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
     </row>
-    <row r="20" spans="1:21" ht="13.2">
+    <row r="20" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>62</v>
       </c>
@@ -1607,7 +1607,7 @@
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
     </row>
-    <row r="21" spans="1:21" ht="13.2">
+    <row r="21" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>64</v>
       </c>
@@ -1656,7 +1656,7 @@
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
     </row>
-    <row r="22" spans="1:21" ht="13.2">
+    <row r="22" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>67</v>
       </c>
@@ -1673,25 +1673,25 @@
         <v>32</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>15</v>
@@ -1705,7 +1705,7 @@
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
     </row>
-    <row r="23" spans="1:21" ht="13.2">
+    <row r="23" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>69</v>
       </c>
@@ -1754,7 +1754,7 @@
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
     </row>
-    <row r="24" spans="1:21" ht="13.2">
+    <row r="24" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>72</v>
       </c>
@@ -1803,7 +1803,7 @@
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
     </row>
-    <row r="25" spans="1:21" ht="13.2">
+    <row r="25" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>74</v>
       </c>
@@ -1852,7 +1852,7 @@
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
     </row>
-    <row r="26" spans="1:21" ht="13.2">
+    <row r="26" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>77</v>
       </c>
@@ -1901,7 +1901,7 @@
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75" customHeight="1">
+    <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Udon Don Bar
Opening hours
</commit_message>
<xml_diff>
--- a/Utown Outlets Opening Hours.xlsx
+++ b/Utown Outlets Opening Hours.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bigch\Desktop\GitHub\NUSUTownTeleBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2ACC835-518B-4B72-AE85-BCED5DC3EE23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D03DF5-F4F4-499D-B527-F8DB83BC31B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$U$26</definedName>
-    <definedName name="Z_DF95D861_E732_478A_9AD9_C6A3452F328A_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$A$1:$F$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$U$27</definedName>
+    <definedName name="Z_DF95D861_E732_478A_9AD9_C6A3452F328A_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$A$1:$F$27</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <customWorkbookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="92">
   <si>
     <t>Store</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t>PH</t>
+  </si>
+  <si>
+    <t>Udon Don Bar</t>
   </si>
 </sst>
 </file>
@@ -593,13 +596,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:U29"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1854,7 +1857,7 @@
     </row>
     <row r="26" spans="1:21" ht="13.2">
       <c r="A26" s="2" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>6</v>
@@ -1866,25 +1869,25 @@
         <v>8</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>20</v>
@@ -1901,11 +1904,60 @@
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75" customHeight="1">
-      <c r="A29" s="5"/>
+    <row r="27" spans="1:21" ht="13.2">
+      <c r="A27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+    </row>
+    <row r="30" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A30" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U26" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:U27" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <customSheetViews>
     <customSheetView guid="{DF95D861-E732-478A-9AD9-C6A3452F328A}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added option for user to show map location for stores.
</commit_message>
<xml_diff>
--- a/Utown Outlets Opening Hours.xlsx
+++ b/Utown Outlets Opening Hours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bigch\Desktop\GitHub\NUSUTownTeleBot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanjin/Desktop/python_projects/telegram_project/NUSUTownTeleBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DDF372-D702-446B-BA55-0B1C6C41D92E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861D75C2-481A-E74F-ACEC-A9F51BFABF2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="118">
   <si>
     <t>Store</t>
   </si>
@@ -303,13 +303,91 @@
   </si>
   <si>
     <t>Udon Don Bar</t>
+  </si>
+  <si>
+    <t>lnglat</t>
+  </si>
+  <si>
+    <t>1.306019,103.772678</t>
+  </si>
+  <si>
+    <t>1.305796,103.773008</t>
+  </si>
+  <si>
+    <t>1.305593,103.773083</t>
+  </si>
+  <si>
+    <t>1.3040592,103.7741032</t>
+  </si>
+  <si>
+    <t>1.3044719,103.7724654</t>
+  </si>
+  <si>
+    <t>1.3039258,103.7735858</t>
+  </si>
+  <si>
+    <t>1.307338,103.7726078</t>
+  </si>
+  <si>
+    <t>1.3045409,103.7727869</t>
+  </si>
+  <si>
+    <t>1.303794,103.7735167</t>
+  </si>
+  <si>
+    <t>1.3050106,103.7723947</t>
+  </si>
+  <si>
+    <t>1.3046285,103.7730182</t>
+  </si>
+  <si>
+    <t>1.3047189,103.7727242</t>
+  </si>
+  <si>
+    <t>1.3044706,103.7724575</t>
+  </si>
+  <si>
+    <t>1.3046387,103.7728153</t>
+  </si>
+  <si>
+    <t>1.3045756,103.7726986</t>
+  </si>
+  <si>
+    <t>1.3054322,103.7728657</t>
+  </si>
+  <si>
+    <t>1.3049764,103.7724652</t>
+  </si>
+  <si>
+    <t>1.3051092,103.7723276</t>
+  </si>
+  <si>
+    <t>1.3045187,103.7728417</t>
+  </si>
+  <si>
+    <t>1.3048207,103.7725693</t>
+  </si>
+  <si>
+    <t>1.3042717,103.7738946</t>
+  </si>
+  <si>
+    <t>1.3038022,103.7738266</t>
+  </si>
+  <si>
+    <t>1.3039101,103.7738303</t>
+  </si>
+  <si>
+    <t>1.3040203,103.7741394</t>
+  </si>
+  <si>
+    <t>1.3047292,103.7725536</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -342,6 +420,10 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -599,38 +681,38 @@
   <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="33.5" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="27.88671875" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" customWidth="1"/>
     <col min="7" max="7" width="27.33203125" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
-    <col min="9" max="9" width="27.44140625" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" customWidth="1"/>
+    <col min="9" max="9" width="27.5" customWidth="1"/>
+    <col min="10" max="10" width="26.5" customWidth="1"/>
     <col min="11" max="11" width="27" customWidth="1"/>
-    <col min="12" max="12" width="27.5546875" customWidth="1"/>
+    <col min="12" max="12" width="27.5" customWidth="1"/>
     <col min="13" max="13" width="26.6640625" customWidth="1"/>
-    <col min="14" max="14" width="31.109375" customWidth="1"/>
-    <col min="15" max="15" width="30.44140625" customWidth="1"/>
-    <col min="16" max="16" width="31.109375" customWidth="1"/>
+    <col min="14" max="14" width="31.1640625" customWidth="1"/>
+    <col min="15" max="15" width="30.5" customWidth="1"/>
+    <col min="16" max="16" width="31.1640625" customWidth="1"/>
     <col min="17" max="17" width="30.6640625" customWidth="1"/>
     <col min="18" max="18" width="29.6640625" customWidth="1"/>
-    <col min="19" max="19" width="30.109375" customWidth="1"/>
-    <col min="20" max="20" width="30.88671875" customWidth="1"/>
-    <col min="21" max="21" width="29.88671875" customWidth="1"/>
+    <col min="19" max="19" width="30.1640625" customWidth="1"/>
+    <col min="20" max="20" width="30.83203125" customWidth="1"/>
+    <col min="21" max="21" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="13.2">
+    <row r="1" spans="1:21" ht="13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -670,7 +752,9 @@
       <c r="M1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="N1" s="1"/>
+      <c r="N1" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -679,7 +763,7 @@
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
     </row>
-    <row r="2" spans="1:21" ht="13.2">
+    <row r="2" spans="1:21" ht="13">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -719,7 +803,9 @@
       <c r="M2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="1"/>
+      <c r="N2" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -728,7 +814,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:21" ht="13.2">
+    <row r="3" spans="1:21" ht="13">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -768,7 +854,9 @@
       <c r="M3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="1"/>
+      <c r="N3" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -777,7 +865,7 @@
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
     </row>
-    <row r="4" spans="1:21" ht="13.2">
+    <row r="4" spans="1:21" ht="13">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -817,7 +905,9 @@
       <c r="M4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="1"/>
+      <c r="N4" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -826,7 +916,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
     </row>
-    <row r="5" spans="1:21" ht="13.2">
+    <row r="5" spans="1:21" ht="13">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -866,7 +956,9 @@
       <c r="M5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N5" s="1"/>
+      <c r="N5" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
@@ -875,7 +967,7 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
     </row>
-    <row r="6" spans="1:21" ht="13.2">
+    <row r="6" spans="1:21" ht="13">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -915,7 +1007,9 @@
       <c r="M6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="1"/>
+      <c r="N6" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -924,7 +1018,7 @@
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
     </row>
-    <row r="7" spans="1:21" ht="13.2">
+    <row r="7" spans="1:21" ht="13">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -964,7 +1058,9 @@
       <c r="M7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="1"/>
+      <c r="N7" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -973,7 +1069,7 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
     </row>
-    <row r="8" spans="1:21" ht="13.2">
+    <row r="8" spans="1:21" ht="13">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
@@ -1013,7 +1109,9 @@
       <c r="M8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="1"/>
+      <c r="N8" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -1022,7 +1120,7 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
     </row>
-    <row r="9" spans="1:21" ht="13.2">
+    <row r="9" spans="1:21" ht="13">
       <c r="A9" s="4" t="s">
         <v>38</v>
       </c>
@@ -1062,7 +1160,9 @@
       <c r="M9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="1"/>
+      <c r="N9" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
@@ -1071,7 +1171,7 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="1:21" ht="13.2">
+    <row r="10" spans="1:21" ht="13">
       <c r="A10" s="2" t="s">
         <v>40</v>
       </c>
@@ -1111,7 +1211,9 @@
       <c r="M10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N10" s="1"/>
+      <c r="N10" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
@@ -1120,7 +1222,7 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="1:21" ht="13.2">
+    <row r="11" spans="1:21" ht="13">
       <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
@@ -1160,7 +1262,9 @@
       <c r="M11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N11" s="1"/>
+      <c r="N11" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
@@ -1169,7 +1273,7 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
     </row>
-    <row r="12" spans="1:21" ht="13.2">
+    <row r="12" spans="1:21" ht="13">
       <c r="A12" s="4" t="s">
         <v>44</v>
       </c>
@@ -1209,7 +1313,9 @@
       <c r="M12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="1"/>
+      <c r="N12" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -1218,7 +1324,7 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="1:21" ht="13.2">
+    <row r="13" spans="1:21" ht="13">
       <c r="A13" s="4" t="s">
         <v>47</v>
       </c>
@@ -1258,7 +1364,9 @@
       <c r="M13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N13" s="1"/>
+      <c r="N13" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
@@ -1267,7 +1375,7 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
     </row>
-    <row r="14" spans="1:21" ht="13.2">
+    <row r="14" spans="1:21" ht="13">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
@@ -1307,7 +1415,9 @@
       <c r="M14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N14" s="1"/>
+      <c r="N14" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
@@ -1316,7 +1426,7 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="1:21" ht="13.2">
+    <row r="15" spans="1:21" ht="13">
       <c r="A15" s="4" t="s">
         <v>51</v>
       </c>
@@ -1356,7 +1466,9 @@
       <c r="M15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N15" s="1"/>
+      <c r="N15" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
@@ -1365,7 +1477,7 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="1:21" ht="13.2">
+    <row r="16" spans="1:21" ht="13">
       <c r="A16" s="2" t="s">
         <v>52</v>
       </c>
@@ -1405,7 +1517,9 @@
       <c r="M16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N16" s="1"/>
+      <c r="N16" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
@@ -1414,7 +1528,7 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
     </row>
-    <row r="17" spans="1:21" ht="13.2">
+    <row r="17" spans="1:21" ht="13">
       <c r="A17" s="2" t="s">
         <v>56</v>
       </c>
@@ -1454,7 +1568,9 @@
       <c r="M17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N17" s="1"/>
+      <c r="N17" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
@@ -1463,7 +1579,7 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
     </row>
-    <row r="18" spans="1:21" ht="13.2">
+    <row r="18" spans="1:21" ht="13">
       <c r="A18" s="4" t="s">
         <v>57</v>
       </c>
@@ -1503,7 +1619,9 @@
       <c r="M18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N18" s="1"/>
+      <c r="N18" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
@@ -1512,7 +1630,7 @@
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
     </row>
-    <row r="19" spans="1:21" ht="13.2">
+    <row r="19" spans="1:21" ht="13">
       <c r="A19" s="2" t="s">
         <v>60</v>
       </c>
@@ -1552,7 +1670,9 @@
       <c r="M19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N19" s="1"/>
+      <c r="N19" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
@@ -1561,7 +1681,7 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
     </row>
-    <row r="20" spans="1:21" ht="13.2">
+    <row r="20" spans="1:21" ht="13">
       <c r="A20" s="2" t="s">
         <v>62</v>
       </c>
@@ -1601,7 +1721,9 @@
       <c r="M20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N20" s="1"/>
+      <c r="N20" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
@@ -1610,7 +1732,7 @@
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
     </row>
-    <row r="21" spans="1:21" ht="13.2">
+    <row r="21" spans="1:21" ht="13">
       <c r="A21" s="4" t="s">
         <v>64</v>
       </c>
@@ -1650,7 +1772,9 @@
       <c r="M21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N21" s="1"/>
+      <c r="N21" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
@@ -1659,7 +1783,7 @@
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
     </row>
-    <row r="22" spans="1:21" ht="13.2">
+    <row r="22" spans="1:21" ht="13">
       <c r="A22" s="2" t="s">
         <v>67</v>
       </c>
@@ -1699,7 +1823,9 @@
       <c r="M22" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="N22" s="1"/>
+      <c r="N22" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
@@ -1708,7 +1834,7 @@
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
     </row>
-    <row r="23" spans="1:21" ht="13.2">
+    <row r="23" spans="1:21" ht="13">
       <c r="A23" s="2" t="s">
         <v>69</v>
       </c>
@@ -1748,7 +1874,9 @@
       <c r="M23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N23" s="1"/>
+      <c r="N23" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
@@ -1757,7 +1885,7 @@
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
     </row>
-    <row r="24" spans="1:21" ht="13.2">
+    <row r="24" spans="1:21" ht="13">
       <c r="A24" s="4" t="s">
         <v>72</v>
       </c>
@@ -1797,7 +1925,9 @@
       <c r="M24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N24" s="1"/>
+      <c r="N24" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
@@ -1806,7 +1936,7 @@
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
     </row>
-    <row r="25" spans="1:21" ht="13.2">
+    <row r="25" spans="1:21" ht="13">
       <c r="A25" s="2" t="s">
         <v>74</v>
       </c>
@@ -1846,7 +1976,9 @@
       <c r="M25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N25" s="1"/>
+      <c r="N25" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
@@ -1855,7 +1987,7 @@
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
     </row>
-    <row r="26" spans="1:21" ht="13.2">
+    <row r="26" spans="1:21" ht="13">
       <c r="A26" s="2" t="s">
         <v>91</v>
       </c>
@@ -1895,7 +2027,9 @@
       <c r="M26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N26" s="1"/>
+      <c r="N26" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
@@ -1904,7 +2038,7 @@
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
     </row>
-    <row r="27" spans="1:21" ht="13.2">
+    <row r="27" spans="1:21" ht="13">
       <c r="A27" s="2" t="s">
         <v>77</v>
       </c>
@@ -1944,7 +2078,9 @@
       <c r="M27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N27" s="1"/>
+      <c r="N27" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
@@ -1964,6 +2100,7 @@
       <autoFilter ref="A1:F26" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactored code to retrieve latitude and longitude with pandas df query instead.
</commit_message>
<xml_diff>
--- a/Utown Outlets Opening Hours.xlsx
+++ b/Utown Outlets Opening Hours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanjin/Desktop/python_projects/telegram_project/NUSUTownTeleBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861D75C2-481A-E74F-ACEC-A9F51BFABF2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9628ECD9-A571-2E45-83AB-3574B5BEF46F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5680" yWindow="3220" windowWidth="23260" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -305,82 +305,82 @@
     <t>Udon Don Bar</t>
   </si>
   <si>
-    <t>lnglat</t>
-  </si>
-  <si>
-    <t>1.306019,103.772678</t>
-  </si>
-  <si>
-    <t>1.305796,103.773008</t>
-  </si>
-  <si>
-    <t>1.305593,103.773083</t>
-  </si>
-  <si>
-    <t>1.3040592,103.7741032</t>
-  </si>
-  <si>
-    <t>1.3044719,103.7724654</t>
-  </si>
-  <si>
-    <t>1.3039258,103.7735858</t>
-  </si>
-  <si>
-    <t>1.307338,103.7726078</t>
-  </si>
-  <si>
-    <t>1.3045409,103.7727869</t>
-  </si>
-  <si>
-    <t>1.303794,103.7735167</t>
-  </si>
-  <si>
-    <t>1.3050106,103.7723947</t>
-  </si>
-  <si>
-    <t>1.3046285,103.7730182</t>
-  </si>
-  <si>
-    <t>1.3047189,103.7727242</t>
-  </si>
-  <si>
-    <t>1.3044706,103.7724575</t>
-  </si>
-  <si>
-    <t>1.3046387,103.7728153</t>
-  </si>
-  <si>
-    <t>1.3045756,103.7726986</t>
-  </si>
-  <si>
-    <t>1.3054322,103.7728657</t>
-  </si>
-  <si>
-    <t>1.3049764,103.7724652</t>
-  </si>
-  <si>
-    <t>1.3051092,103.7723276</t>
-  </si>
-  <si>
-    <t>1.3045187,103.7728417</t>
-  </si>
-  <si>
-    <t>1.3048207,103.7725693</t>
-  </si>
-  <si>
-    <t>1.3042717,103.7738946</t>
-  </si>
-  <si>
-    <t>1.3038022,103.7738266</t>
-  </si>
-  <si>
-    <t>1.3039101,103.7738303</t>
-  </si>
-  <si>
-    <t>1.3040203,103.7741394</t>
-  </si>
-  <si>
-    <t>1.3047292,103.7725536</t>
+    <t>1.3044719</t>
+  </si>
+  <si>
+    <t>1.307338</t>
+  </si>
+  <si>
+    <t>1.3045409</t>
+  </si>
+  <si>
+    <t>1.303794</t>
+  </si>
+  <si>
+    <t>1.306019</t>
+  </si>
+  <si>
+    <t>1.3050106</t>
+  </si>
+  <si>
+    <t>1.3039258</t>
+  </si>
+  <si>
+    <t>1.3046285</t>
+  </si>
+  <si>
+    <t>1.3047189</t>
+  </si>
+  <si>
+    <t>1.3044706</t>
+  </si>
+  <si>
+    <t>1.3051092</t>
+  </si>
+  <si>
+    <t>1.3040592</t>
+  </si>
+  <si>
+    <t>1.305593</t>
+  </si>
+  <si>
+    <t>1.3045187</t>
+  </si>
+  <si>
+    <t>1.3048207</t>
+  </si>
+  <si>
+    <t>1.305796</t>
+  </si>
+  <si>
+    <t>1.3042717</t>
+  </si>
+  <si>
+    <t>1.3046387</t>
+  </si>
+  <si>
+    <t>1.3045756</t>
+  </si>
+  <si>
+    <t>1.3054322</t>
+  </si>
+  <si>
+    <t>1.3049764</t>
+  </si>
+  <si>
+    <t>1.3039101</t>
+  </si>
+  <si>
+    <t>1.3040203</t>
+  </si>
+  <si>
+    <t>1.3047292</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
   </si>
 </sst>
 </file>
@@ -452,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -460,6 +460,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,10 +683,10 @@
   <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N18" sqref="N18"/>
+      <selection pane="bottomRight" activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -702,7 +704,7 @@
     <col min="11" max="11" width="27" customWidth="1"/>
     <col min="12" max="12" width="27.5" customWidth="1"/>
     <col min="13" max="13" width="26.6640625" customWidth="1"/>
-    <col min="14" max="14" width="31.1640625" customWidth="1"/>
+    <col min="14" max="14" width="31.1640625" style="8" customWidth="1"/>
     <col min="15" max="15" width="30.5" customWidth="1"/>
     <col min="16" max="16" width="31.1640625" customWidth="1"/>
     <col min="17" max="17" width="30.6640625" customWidth="1"/>
@@ -752,10 +754,12 @@
       <c r="M1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="O1" s="1"/>
+      <c r="N1" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -803,10 +807,12 @@
       <c r="M2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="O2" s="1"/>
+      <c r="N2" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="O2" s="7">
+        <v>103.7724654</v>
+      </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -854,10 +860,12 @@
       <c r="M3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="O3" s="1"/>
+      <c r="N3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="O3" s="7">
+        <v>103.7726078</v>
+      </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -905,10 +913,12 @@
       <c r="M4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="O4" s="1"/>
+      <c r="N4" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="O4" s="7">
+        <v>103.7727869</v>
+      </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -956,10 +966,12 @@
       <c r="M5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="O5" s="1"/>
+      <c r="N5" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="O5" s="7">
+        <v>103.7735167</v>
+      </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
@@ -1007,10 +1019,12 @@
       <c r="M6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="O6" s="1"/>
+      <c r="N6" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="O6" s="7">
+        <v>103.772678</v>
+      </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -1058,10 +1072,12 @@
       <c r="M7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="O7" s="1"/>
+      <c r="N7" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O7" s="7">
+        <v>103.77239470000001</v>
+      </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
@@ -1109,10 +1125,12 @@
       <c r="M8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="O8" s="1"/>
+      <c r="O8" s="7">
+        <v>103.77358580000001</v>
+      </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -1160,10 +1178,12 @@
       <c r="M9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="O9" s="1"/>
+      <c r="N9" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="O9" s="7">
+        <v>103.7730182</v>
+      </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -1211,10 +1231,12 @@
       <c r="M10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N10" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="O10" s="1"/>
+      <c r="N10" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="O10" s="7">
+        <v>103.7727242</v>
+      </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
@@ -1262,10 +1284,12 @@
       <c r="M11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N11" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="O11" s="1"/>
+      <c r="N11" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="O11" s="7">
+        <v>103.7724575</v>
+      </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
@@ -1313,10 +1337,12 @@
       <c r="M12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="O12" s="1"/>
+      <c r="N12" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="O12" s="7">
+        <v>103.7723276</v>
+      </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -1364,10 +1390,12 @@
       <c r="M13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="O13" s="1"/>
+      <c r="N13" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="O13" s="7">
+        <v>103.7741032</v>
+      </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
@@ -1415,10 +1443,12 @@
       <c r="M14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O14" s="1"/>
+      <c r="N14" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="O14" s="7">
+        <v>103.773083</v>
+      </c>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
@@ -1466,10 +1496,12 @@
       <c r="M15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="O15" s="1"/>
+      <c r="N15" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="O15" s="7">
+        <v>103.7728417</v>
+      </c>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -1517,10 +1549,12 @@
       <c r="M16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N16" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="O16" s="1"/>
+      <c r="N16" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="O16" s="7">
+        <v>103.7725693</v>
+      </c>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
@@ -1568,10 +1602,12 @@
       <c r="M17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N17" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="O17" s="1"/>
+      <c r="N17" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="O17" s="7">
+        <v>103.773008</v>
+      </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
@@ -1619,10 +1655,12 @@
       <c r="M18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N18" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="O18" s="1"/>
+      <c r="N18" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="O18" s="7">
+        <v>103.7730182</v>
+      </c>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -1670,10 +1708,12 @@
       <c r="M19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N19" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="O19" s="1"/>
+      <c r="N19" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="O19" s="7">
+        <v>103.77389460000001</v>
+      </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
@@ -1721,10 +1761,12 @@
       <c r="M20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N20" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="O20" s="1"/>
+      <c r="N20" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="O20" s="7">
+        <v>103.7728153</v>
+      </c>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
@@ -1772,10 +1814,12 @@
       <c r="M21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N21" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="O21" s="1"/>
+      <c r="N21" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="O21" s="7">
+        <v>103.7726986</v>
+      </c>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
@@ -1823,10 +1867,12 @@
       <c r="M22" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="N22" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="O22" s="1"/>
+      <c r="N22" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="O22" s="7">
+        <v>103.7728657</v>
+      </c>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
@@ -1874,10 +1920,12 @@
       <c r="M23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N23" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="O23" s="1"/>
+      <c r="N23" s="7">
+        <v>1.3038022</v>
+      </c>
+      <c r="O23" s="7">
+        <v>103.77382660000001</v>
+      </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
@@ -1925,10 +1973,12 @@
       <c r="M24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N24" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="O24" s="1"/>
+      <c r="N24" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="O24" s="7">
+        <v>103.7724652</v>
+      </c>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
@@ -1976,10 +2026,12 @@
       <c r="M25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N25" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="O25" s="1"/>
+      <c r="N25" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="O25" s="7">
+        <v>103.7738303</v>
+      </c>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
@@ -2027,10 +2079,12 @@
       <c r="M26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N26" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="O26" s="1"/>
+      <c r="N26" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="O26" s="7">
+        <v>103.7741394</v>
+      </c>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
@@ -2078,10 +2132,12 @@
       <c r="M27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N27" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="O27" s="1"/>
+      <c r="N27" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="O27" s="7">
+        <v>103.77255359999999</v>
+      </c>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
@@ -2103,5 +2159,8 @@
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="N27 N2:N26" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated to use google maps link instead of latitude and longitude.
</commit_message>
<xml_diff>
--- a/Utown Outlets Opening Hours.xlsx
+++ b/Utown Outlets Opening Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanjin/Desktop/python_projects/telegram_project/NUSUTownTeleBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9628ECD9-A571-2E45-83AB-3574B5BEF46F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304DABCB-1FFF-5D47-B307-E497592DB7FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5680" yWindow="3220" windowWidth="23260" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$U$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$27</definedName>
     <definedName name="Z_DF95D861_E732_478A_9AD9_C6A3452F328A_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$A$1:$F$27</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -305,89 +305,89 @@
     <t>Udon Don Bar</t>
   </si>
   <si>
-    <t>1.3044719</t>
-  </si>
-  <si>
-    <t>1.307338</t>
-  </si>
-  <si>
-    <t>1.3045409</t>
-  </si>
-  <si>
-    <t>1.303794</t>
-  </si>
-  <si>
-    <t>1.306019</t>
-  </si>
-  <si>
-    <t>1.3050106</t>
-  </si>
-  <si>
-    <t>1.3039258</t>
-  </si>
-  <si>
-    <t>1.3046285</t>
-  </si>
-  <si>
-    <t>1.3047189</t>
-  </si>
-  <si>
-    <t>1.3044706</t>
-  </si>
-  <si>
-    <t>1.3051092</t>
-  </si>
-  <si>
-    <t>1.3040592</t>
-  </si>
-  <si>
-    <t>1.305593</t>
-  </si>
-  <si>
-    <t>1.3045187</t>
-  </si>
-  <si>
-    <t>1.3048207</t>
-  </si>
-  <si>
-    <t>1.305796</t>
-  </si>
-  <si>
-    <t>1.3042717</t>
-  </si>
-  <si>
-    <t>1.3046387</t>
-  </si>
-  <si>
-    <t>1.3045756</t>
-  </si>
-  <si>
-    <t>1.3054322</t>
-  </si>
-  <si>
-    <t>1.3049764</t>
-  </si>
-  <si>
-    <t>1.3039101</t>
-  </si>
-  <si>
-    <t>1.3040203</t>
-  </si>
-  <si>
-    <t>1.3047292</t>
-  </si>
-  <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
+    <t>Maps</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/poLHvL9UBWTKNb1G8</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/VHvmVFozaqfZXvbE9</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/r9G6Uno2YAgA4LEg7</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/nSg9FFxLRmcBg3Z18</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/eUHfiCPwgfRi7gae6</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/VkjREyA6zNJcW6dL6</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/uB7VXqb4VMsjR74n8</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/tWDMyawW21QqTiaU6</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/zWZDt7W5PCc5xtP89</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/yHzn96oNnfMyrZP4A</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/NctRQb1oQU2F7XcC9</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/TVoeSWVHrYohc9Ra6</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/rgv2MC5ffMEy2F4L6</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/D4Ptn8UrNXR4Bbkj8</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/M5vbmKxtnagZ3Jp66</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/mH8Z3SF8rH3Ynj7MA</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/9Ts4xERRLZsuQzVE8</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/d4YmuG9wxEysZxWJ8</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/tyeThCtvT7YVXXux8</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/knUTS44tkG36Ppdt7</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/YkL7HMAym5shWYoAA</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/pgfRRWX9ei9EKHHdA</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/S4GX5oriaQ5forUB9</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/fCPpAtTWQ5icqfT66</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/43LkWYeDxApzgXTH8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -425,6 +425,12 @@
       <sz val="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -449,10 +455,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -460,10 +467,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -680,13 +687,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:U30"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P18" sqref="P18"/>
+      <selection pane="bottomRight" activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -704,17 +711,15 @@
     <col min="11" max="11" width="27" customWidth="1"/>
     <col min="12" max="12" width="27.5" customWidth="1"/>
     <col min="13" max="13" width="26.6640625" customWidth="1"/>
-    <col min="14" max="14" width="31.1640625" style="8" customWidth="1"/>
-    <col min="15" max="15" width="30.5" customWidth="1"/>
-    <col min="16" max="16" width="31.1640625" customWidth="1"/>
-    <col min="17" max="17" width="30.6640625" customWidth="1"/>
-    <col min="18" max="18" width="29.6640625" customWidth="1"/>
-    <col min="19" max="19" width="30.1640625" customWidth="1"/>
-    <col min="20" max="20" width="30.83203125" customWidth="1"/>
-    <col min="21" max="21" width="29.83203125" customWidth="1"/>
+    <col min="14" max="14" width="31.1640625" customWidth="1"/>
+    <col min="15" max="15" width="30.6640625" customWidth="1"/>
+    <col min="16" max="16" width="29.6640625" customWidth="1"/>
+    <col min="17" max="17" width="30.1640625" customWidth="1"/>
+    <col min="18" max="18" width="30.83203125" customWidth="1"/>
+    <col min="19" max="19" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="13">
+    <row r="1" spans="1:19" ht="13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -754,20 +759,16 @@
       <c r="M1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="N1" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>117</v>
-      </c>
+      <c r="N1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-    </row>
-    <row r="2" spans="1:21" ht="13">
+    </row>
+    <row r="2" spans="1:19" ht="13">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -807,20 +808,16 @@
       <c r="M2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="O2" s="7">
-        <v>103.7724654</v>
-      </c>
+      <c r="N2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-    </row>
-    <row r="3" spans="1:21" ht="13">
+    </row>
+    <row r="3" spans="1:19" ht="13">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -860,20 +857,16 @@
       <c r="M3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="O3" s="7">
-        <v>103.7726078</v>
-      </c>
+      <c r="N3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-    </row>
-    <row r="4" spans="1:21" ht="13">
+    </row>
+    <row r="4" spans="1:19" ht="13">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -913,20 +906,16 @@
       <c r="M4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="O4" s="7">
-        <v>103.7727869</v>
-      </c>
+      <c r="N4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-    </row>
-    <row r="5" spans="1:21" ht="13">
+    </row>
+    <row r="5" spans="1:19" ht="13">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -967,19 +956,15 @@
         <v>15</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="O5" s="7">
-        <v>103.7735167</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-    </row>
-    <row r="6" spans="1:21" ht="13">
+    </row>
+    <row r="6" spans="1:19" ht="13">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -1019,20 +1004,16 @@
       <c r="M6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="O6" s="7">
-        <v>103.772678</v>
-      </c>
+      <c r="N6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-    </row>
-    <row r="7" spans="1:21" ht="13">
+    </row>
+    <row r="7" spans="1:19" ht="13">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -1072,20 +1053,16 @@
       <c r="M7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="O7" s="7">
-        <v>103.77239470000001</v>
-      </c>
+      <c r="N7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-    </row>
-    <row r="8" spans="1:21" ht="13">
+    </row>
+    <row r="8" spans="1:19" ht="13">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
@@ -1126,19 +1103,15 @@
         <v>15</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O8" s="7">
-        <v>103.77358580000001</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-    </row>
-    <row r="9" spans="1:21" ht="13">
+    </row>
+    <row r="9" spans="1:19" ht="13">
       <c r="A9" s="4" t="s">
         <v>38</v>
       </c>
@@ -1178,20 +1151,16 @@
       <c r="M9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="O9" s="7">
-        <v>103.7730182</v>
-      </c>
+      <c r="N9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-    </row>
-    <row r="10" spans="1:21" ht="13">
+    </row>
+    <row r="10" spans="1:19" ht="13">
       <c r="A10" s="2" t="s">
         <v>40</v>
       </c>
@@ -1231,20 +1200,16 @@
       <c r="M10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N10" s="7" t="s">
+      <c r="N10" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="O10" s="7">
-        <v>103.7727242</v>
-      </c>
+      <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-    </row>
-    <row r="11" spans="1:21" ht="13">
+    </row>
+    <row r="11" spans="1:19" ht="13">
       <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
@@ -1284,20 +1249,16 @@
       <c r="M11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N11" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="O11" s="7">
-        <v>103.7724575</v>
-      </c>
+      <c r="N11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-    </row>
-    <row r="12" spans="1:21" ht="13">
+    </row>
+    <row r="12" spans="1:19" ht="13">
       <c r="A12" s="4" t="s">
         <v>44</v>
       </c>
@@ -1337,20 +1298,16 @@
       <c r="M12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="O12" s="7">
-        <v>103.7723276</v>
-      </c>
+      <c r="N12" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-    </row>
-    <row r="13" spans="1:21" ht="13">
+    </row>
+    <row r="13" spans="1:19" ht="13">
       <c r="A13" s="4" t="s">
         <v>47</v>
       </c>
@@ -1390,20 +1347,16 @@
       <c r="M13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N13" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="O13" s="7">
-        <v>103.7741032</v>
-      </c>
+      <c r="N13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-    </row>
-    <row r="14" spans="1:21" ht="13">
+    </row>
+    <row r="14" spans="1:19" ht="13">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
@@ -1443,20 +1396,16 @@
       <c r="M14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N14" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="O14" s="7">
-        <v>103.773083</v>
-      </c>
+      <c r="N14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-    </row>
-    <row r="15" spans="1:21" ht="13">
+    </row>
+    <row r="15" spans="1:19" ht="13">
       <c r="A15" s="4" t="s">
         <v>51</v>
       </c>
@@ -1496,20 +1445,16 @@
       <c r="M15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N15" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="O15" s="7">
-        <v>103.7728417</v>
-      </c>
+      <c r="N15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-    </row>
-    <row r="16" spans="1:21" ht="13">
+    </row>
+    <row r="16" spans="1:19" ht="13">
       <c r="A16" s="2" t="s">
         <v>52</v>
       </c>
@@ -1549,20 +1494,16 @@
       <c r="M16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N16" s="7" t="s">
+      <c r="N16" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="O16" s="7">
-        <v>103.7725693</v>
-      </c>
+      <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-    </row>
-    <row r="17" spans="1:21" ht="13">
+    </row>
+    <row r="17" spans="1:19" ht="13">
       <c r="A17" s="2" t="s">
         <v>56</v>
       </c>
@@ -1602,20 +1543,16 @@
       <c r="M17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N17" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="O17" s="7">
-        <v>103.773008</v>
-      </c>
+      <c r="N17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-    </row>
-    <row r="18" spans="1:21" ht="13">
+    </row>
+    <row r="18" spans="1:19" ht="13">
       <c r="A18" s="4" t="s">
         <v>57</v>
       </c>
@@ -1655,20 +1592,16 @@
       <c r="M18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N18" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="O18" s="7">
-        <v>103.7730182</v>
-      </c>
+      <c r="N18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-    </row>
-    <row r="19" spans="1:21" ht="13">
+    </row>
+    <row r="19" spans="1:19" ht="13">
       <c r="A19" s="2" t="s">
         <v>60</v>
       </c>
@@ -1708,20 +1641,16 @@
       <c r="M19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N19" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="O19" s="7">
-        <v>103.77389460000001</v>
-      </c>
+      <c r="N19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-    </row>
-    <row r="20" spans="1:21" ht="13">
+    </row>
+    <row r="20" spans="1:19" ht="13">
       <c r="A20" s="2" t="s">
         <v>62</v>
       </c>
@@ -1761,20 +1690,16 @@
       <c r="M20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N20" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="O20" s="7">
-        <v>103.7728153</v>
-      </c>
+      <c r="N20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-    </row>
-    <row r="21" spans="1:21" ht="13">
+    </row>
+    <row r="21" spans="1:19" ht="13">
       <c r="A21" s="4" t="s">
         <v>64</v>
       </c>
@@ -1814,20 +1739,16 @@
       <c r="M21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N21" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="O21" s="7">
-        <v>103.7726986</v>
-      </c>
+      <c r="N21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-    </row>
-    <row r="22" spans="1:21" ht="13">
+    </row>
+    <row r="22" spans="1:19" ht="13">
       <c r="A22" s="2" t="s">
         <v>67</v>
       </c>
@@ -1867,20 +1788,16 @@
       <c r="M22" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="N22" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="O22" s="7">
-        <v>103.7728657</v>
-      </c>
+      <c r="N22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-    </row>
-    <row r="23" spans="1:21" ht="13">
+    </row>
+    <row r="23" spans="1:19" ht="13">
       <c r="A23" s="2" t="s">
         <v>69</v>
       </c>
@@ -1920,20 +1837,16 @@
       <c r="M23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N23" s="7">
-        <v>1.3038022</v>
-      </c>
-      <c r="O23" s="7">
-        <v>103.77382660000001</v>
-      </c>
+      <c r="N23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-    </row>
-    <row r="24" spans="1:21" ht="13">
+    </row>
+    <row r="24" spans="1:19" ht="13">
       <c r="A24" s="4" t="s">
         <v>72</v>
       </c>
@@ -1973,20 +1886,16 @@
       <c r="M24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N24" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="O24" s="7">
-        <v>103.7724652</v>
-      </c>
+      <c r="N24" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-    </row>
-    <row r="25" spans="1:21" ht="13">
+    </row>
+    <row r="25" spans="1:19" ht="13">
       <c r="A25" s="2" t="s">
         <v>74</v>
       </c>
@@ -2026,20 +1935,16 @@
       <c r="M25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N25" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="O25" s="7">
-        <v>103.7738303</v>
-      </c>
+      <c r="N25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-    </row>
-    <row r="26" spans="1:21" ht="13">
+    </row>
+    <row r="26" spans="1:19" ht="13">
       <c r="A26" s="2" t="s">
         <v>91</v>
       </c>
@@ -2079,20 +1984,16 @@
       <c r="M26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N26" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="O26" s="7">
-        <v>103.7741394</v>
-      </c>
+      <c r="N26" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
-    </row>
-    <row r="27" spans="1:21" ht="13">
+    </row>
+    <row r="27" spans="1:19" ht="13">
       <c r="A27" s="2" t="s">
         <v>77</v>
       </c>
@@ -2132,24 +2033,20 @@
       <c r="M27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N27" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="O27" s="7">
-        <v>103.77255359999999</v>
-      </c>
+      <c r="N27" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
-    </row>
-    <row r="30" spans="1:21" ht="15.75" customHeight="1">
+    </row>
+    <row r="30" spans="1:19" ht="15.75" customHeight="1">
       <c r="A30" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U27" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:S27" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <customSheetViews>
     <customSheetView guid="{DF95D861-E732-478A-9AD9-C6A3452F328A}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2157,10 +2054,10 @@
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="6" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="N8" r:id="rId1" xr:uid="{905360E2-7AA7-C34C-AEF5-9E979868A121}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="N27 N2:N26" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>